<commit_message>
[CODE OPT] - Added closing of app and config values
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\Projects\RPA Challenge\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath Repos\TestUipath\RPA-Challenge\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFAB1A0-3EDB-4139-AC0F-13EA90373438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA097B-1B07-4035-87D0-A89E59FB4F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>https://rpachallenge.com/</t>
+  </si>
+  <si>
+    <t>WorkbookFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\challenge.xlsx</t>
   </si>
 </sst>
 </file>
@@ -630,9 +642,21 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B7" s="5"/>
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1625,8 +1649,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{C0F655FB-5342-4B5A-983D-1C14E80F427C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>